<commit_message>
Update: Couriers and shipments
</commit_message>
<xml_diff>
--- a/database/imports/products.xlsx
+++ b/database/imports/products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ED\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\web-projects\laravue-erp\database\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FABE434-39A5-4C67-BB32-8060A8828617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5203DC0B-D533-43EB-A0A1-301BA4CA5B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1621,7 +1621,7 @@
     <t>products/avatars/image185.png</t>
   </si>
   <si>
-    <t>Kanzen Homes Bulacan</t>
+    <t>KANZEN HOME BALIUAG</t>
   </si>
 </sst>
 </file>
@@ -1992,13 +1992,14 @@
   <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>